<commit_message>
updated E6600 from IDEAcenter
</commit_message>
<xml_diff>
--- a/3Dmark/3dmark.xlsx
+++ b/3Dmark/3dmark.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\OneDrive\Documents\GitHub\benchmark\3Dmark\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Software\Library\Github\benchmark\3Dmark\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="457" documentId="11_AD4DB114E441178AC67DF4EBEE97E408693EDF27" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{8939B046-BF56-4E07-B81F-CF1A4ED6EB37}"/>
   <bookViews>
-    <workbookView xWindow="810" yWindow="8340" windowWidth="26685" windowHeight="11895" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="810" yWindow="8340" windowWidth="26690" windowHeight="11900" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="raw" sheetId="1" r:id="rId1"/>
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="230" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="159">
   <si>
     <t>Grafikkarte</t>
   </si>
@@ -495,12 +494,21 @@
   </si>
   <si>
     <t>night_raid</t>
+  </si>
+  <si>
+    <t>Testbench Ideacenter</t>
+  </si>
+  <si>
+    <t>Pentium E6600</t>
+  </si>
+  <si>
+    <t>nVidia 9600 GSO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -983,26 +991,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J3" sqref="J3:J18"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" customWidth="1"/>
+    <col min="1" max="1" width="27.7265625" customWidth="1"/>
     <col min="2" max="2" width="26" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.26953125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
-    <col min="5" max="8" width="8.42578125" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" customWidth="1"/>
-    <col min="10" max="10" width="22.42578125" customWidth="1"/>
-    <col min="11" max="11" width="22.140625" customWidth="1"/>
+    <col min="5" max="8" width="8.453125" customWidth="1"/>
+    <col min="9" max="9" width="28.54296875" customWidth="1"/>
+    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="11" max="11" width="22.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A1" s="21" t="s">
         <v>72</v>
       </c>
@@ -1033,7 +1041,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" s="21"/>
       <c r="B2" s="21"/>
       <c r="C2" s="2" t="s">
@@ -1060,7 +1068,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
         <v>11</v>
       </c>
@@ -1085,7 +1093,7 @@
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
         <v>15</v>
       </c>
@@ -1114,7 +1122,7 @@
       <c r="J4" s="1"/>
       <c r="K4" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>18</v>
       </c>
@@ -1143,7 +1151,7 @@
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
@@ -1172,7 +1180,7 @@
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
         <v>23</v>
       </c>
@@ -1197,7 +1205,7 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>25</v>
       </c>
@@ -1226,7 +1234,7 @@
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>28</v>
       </c>
@@ -1261,7 +1269,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" s="4" t="s">
         <v>34</v>
       </c>
@@ -1292,7 +1300,7 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" s="4" t="s">
         <v>38</v>
       </c>
@@ -1319,7 +1327,7 @@
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" s="4" t="s">
         <v>41</v>
       </c>
@@ -1350,7 +1358,7 @@
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
@@ -1383,7 +1391,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
         <v>50</v>
       </c>
@@ -1418,7 +1426,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
         <v>56</v>
       </c>
@@ -1453,7 +1461,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
         <v>62</v>
       </c>
@@ -1484,7 +1492,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
         <v>62</v>
       </c>
@@ -1511,7 +1519,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
         <v>62</v>
       </c>
@@ -1561,25 +1569,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9849F7C7-26D4-4D1D-82D0-DFED8D9A7AB7}">
-  <dimension ref="A1:V23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:V24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R20" sqref="R20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="6" width="6.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="15" width="8.28515625" customWidth="1"/>
+    <col min="1" max="1" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.26953125" customWidth="1"/>
+    <col min="5" max="6" width="6.54296875" customWidth="1"/>
+    <col min="7" max="7" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="15" width="8.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
       <c r="D1" s="11"/>
       <c r="E1" s="23" t="s">
         <v>79</v>
@@ -1613,7 +1621,7 @@
       <c r="T1" s="22"/>
       <c r="U1" s="22"/>
     </row>
-    <row r="2" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
         <v>73</v>
       </c>
@@ -1678,7 +1686,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>81</v>
       </c>
@@ -1714,7 +1722,7 @@
       <c r="S3" s="8"/>
       <c r="U3" s="11"/>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>104</v>
       </c>
@@ -1754,7 +1762,7 @@
       <c r="S4" s="8"/>
       <c r="U4" s="11"/>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>142</v>
       </c>
@@ -1801,7 +1809,7 @@
       <c r="S5" s="8"/>
       <c r="U5" s="11"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>144</v>
       </c>
@@ -1835,7 +1843,7 @@
       <c r="S6" s="8"/>
       <c r="U6" s="11"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>103</v>
       </c>
@@ -1886,7 +1894,7 @@
       <c r="S7" s="8"/>
       <c r="U7" s="11"/>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -1933,7 +1941,7 @@
       <c r="S8" s="8"/>
       <c r="U8" s="11"/>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>141</v>
       </c>
@@ -1991,7 +1999,7 @@
       <c r="S9" s="8"/>
       <c r="U9" s="11"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>102</v>
       </c>
@@ -2042,7 +2050,7 @@
       <c r="S10" s="8"/>
       <c r="U10" s="11"/>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>143</v>
       </c>
@@ -2089,7 +2097,7 @@
       <c r="S11" s="8"/>
       <c r="U11" s="11"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -2140,7 +2148,7 @@
       <c r="S12" s="8"/>
       <c r="U12" s="11"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>101</v>
       </c>
@@ -2198,7 +2206,7 @@
       <c r="S13" s="8"/>
       <c r="U13" s="11"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>147</v>
       </c>
@@ -2243,7 +2251,7 @@
       <c r="S14" s="8"/>
       <c r="U14" s="11"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>103</v>
       </c>
@@ -2299,7 +2307,7 @@
       <c r="S15" s="8"/>
       <c r="U15" s="11"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>100</v>
       </c>
@@ -2357,7 +2365,7 @@
       <c r="S16" s="8"/>
       <c r="U16" s="11"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>145</v>
       </c>
@@ -2402,320 +2410,291 @@
       <c r="S17" s="8"/>
       <c r="U17" s="11"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>148</v>
+        <v>156</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>157</v>
       </c>
       <c r="C18" s="7">
-        <v>3.2</v>
+        <v>3.06</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="14">
-        <v>1636</v>
-      </c>
-      <c r="F18" s="11">
-        <v>195</v>
-      </c>
-      <c r="G18" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="H18" s="14">
-        <v>32919</v>
-      </c>
-      <c r="I18" s="11">
-        <v>2374</v>
-      </c>
-      <c r="J18" s="14">
-        <v>17129</v>
-      </c>
-      <c r="K18" s="11">
-        <v>21693</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="E18" s="14"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="15"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="11"/>
       <c r="L18">
-        <v>11357</v>
+        <v>8052</v>
       </c>
       <c r="M18">
-        <v>4001</v>
+        <v>3753</v>
       </c>
       <c r="N18">
-        <v>4992</v>
+        <v>3625</v>
       </c>
       <c r="O18" s="11">
-        <v>4831</v>
-      </c>
-      <c r="P18" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="Q18">
-        <v>5404</v>
-      </c>
-      <c r="R18" s="11">
-        <v>11146</v>
-      </c>
+        <v>1873</v>
+      </c>
+      <c r="P18" s="8"/>
+      <c r="R18" s="11"/>
       <c r="S18" s="8"/>
       <c r="U18" s="11"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>148</v>
+      </c>
+      <c r="B19" t="s">
+        <v>95</v>
+      </c>
+      <c r="C19" s="7">
+        <v>3.2</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="E19" s="14">
+        <v>1636</v>
+      </c>
+      <c r="F19" s="11">
+        <v>195</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="14">
+        <v>32919</v>
+      </c>
+      <c r="I19" s="11">
+        <v>2374</v>
+      </c>
+      <c r="J19" s="14">
+        <v>17129</v>
+      </c>
+      <c r="K19" s="11">
+        <v>21693</v>
+      </c>
+      <c r="L19">
+        <v>11357</v>
+      </c>
+      <c r="M19">
+        <v>4001</v>
+      </c>
+      <c r="N19">
+        <v>4992</v>
+      </c>
+      <c r="O19" s="11">
+        <v>4831</v>
+      </c>
+      <c r="P19" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q19">
+        <v>5404</v>
+      </c>
+      <c r="R19" s="11">
+        <v>11146</v>
+      </c>
+      <c r="S19" s="8"/>
+      <c r="U19" s="11"/>
+    </row>
+    <row r="20" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
         <v>125</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>126</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C20" s="7">
         <v>2.6</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>128</v>
       </c>
-      <c r="E19" s="14">
+      <c r="E20" s="14">
         <v>4315</v>
       </c>
-      <c r="F19" s="11">
+      <c r="F20" s="11">
         <v>477</v>
       </c>
-      <c r="G19" s="15">
+      <c r="G20" s="15">
         <v>39582</v>
       </c>
-      <c r="H19" s="14">
+      <c r="H20" s="14">
         <v>30577</v>
       </c>
-      <c r="I19" s="11">
+      <c r="I20" s="11">
         <v>326</v>
       </c>
-      <c r="J19" s="14">
+      <c r="J20" s="14">
         <v>16656</v>
       </c>
-      <c r="K19" s="11">
+      <c r="K20" s="11">
         <v>1313</v>
       </c>
-      <c r="L19" s="19">
+      <c r="L20" s="19">
         <v>12732</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M20" s="19">
         <v>5001</v>
       </c>
-      <c r="N19" s="19">
+      <c r="N20" s="19">
         <v>4887</v>
       </c>
-      <c r="O19" s="11">
+      <c r="O20" s="11">
         <v>6138</v>
       </c>
-      <c r="P19" s="8" t="s">
+      <c r="P20" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="Q19" s="19">
+      <c r="Q20" s="19">
         <v>7794</v>
       </c>
-      <c r="R19" s="11">
+      <c r="R20" s="11">
         <v>17676</v>
       </c>
-      <c r="S19" s="8" t="s">
+      <c r="S20" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="T19">
+      <c r="T20">
         <v>2004</v>
       </c>
-      <c r="U19" s="11">
+      <c r="U20" s="11">
         <v>6531</v>
       </c>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
         <v>149</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>98</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C21" s="7">
         <v>2.67</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="E20" s="14"/>
-      <c r="F20" s="11"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="14"/>
-      <c r="I20" s="11"/>
-      <c r="J20" s="14">
+      <c r="E21" s="14"/>
+      <c r="F21" s="11"/>
+      <c r="G21" s="15"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="14">
         <v>23055</v>
       </c>
-      <c r="K20" s="11">
+      <c r="K21" s="11">
         <v>22128</v>
       </c>
-      <c r="L20">
+      <c r="L21">
         <v>17083</v>
       </c>
-      <c r="M20">
+      <c r="M21">
         <v>6631</v>
       </c>
-      <c r="N20">
+      <c r="N21">
         <v>7194</v>
       </c>
-      <c r="O20" s="11">
+      <c r="O21" s="11">
         <v>6416</v>
       </c>
-      <c r="P20" s="8" t="s">
+      <c r="P21" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="Q20">
+      <c r="Q21">
         <v>11336</v>
       </c>
-      <c r="R20" s="11">
+      <c r="R21" s="11">
         <v>33177</v>
       </c>
-      <c r="S20" s="8" t="s">
+      <c r="S21" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="T20">
+      <c r="T21">
         <v>2830</v>
       </c>
-      <c r="U20" s="11">
+      <c r="U21" s="11">
         <v>8632</v>
       </c>
-      <c r="V20" s="19"/>
-    </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="V21" s="19"/>
+    </row>
+    <row r="22" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
         <v>96</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B22" t="s">
         <v>82</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C22" s="7">
         <v>2.7</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D22" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E22" s="14">
         <v>4307</v>
       </c>
-      <c r="F21" s="11">
+      <c r="F22" s="11">
         <v>475</v>
       </c>
-      <c r="G21" s="15">
+      <c r="G22" s="15">
         <v>62894</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H22" s="14">
         <v>61569</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I22" s="11">
         <v>353</v>
       </c>
-      <c r="J21" s="14">
+      <c r="J22" s="14">
         <v>31804</v>
       </c>
-      <c r="K21" s="11">
+      <c r="K22" s="11">
         <v>1136</v>
       </c>
-      <c r="L21">
+      <c r="L22">
         <v>24977</v>
       </c>
-      <c r="M21">
+      <c r="M22">
         <v>9937</v>
       </c>
-      <c r="N21">
+      <c r="N22">
         <v>11437</v>
       </c>
-      <c r="O21" s="11">
+      <c r="O22" s="11">
         <v>7296</v>
       </c>
-      <c r="P21" s="8" t="s">
+      <c r="P22" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="Q21">
+      <c r="Q22">
         <v>16638</v>
       </c>
-      <c r="R21" s="11">
+      <c r="R22" s="11">
         <v>25670</v>
       </c>
-      <c r="S21" s="8" t="s">
+      <c r="S22" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="T21">
+      <c r="T22">
         <v>4242</v>
       </c>
-      <c r="U21" s="11">
+      <c r="U22" s="11">
         <v>9030</v>
       </c>
-      <c r="V21" s="19"/>
-    </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="V22" s="19"/>
+    </row>
+    <row r="23" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
         <v>151</v>
-      </c>
-      <c r="B22" t="s">
-        <v>98</v>
-      </c>
-      <c r="C22" s="7">
-        <v>2.67</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="E22" s="14">
-        <v>4296</v>
-      </c>
-      <c r="F22" s="11">
-        <v>476</v>
-      </c>
-      <c r="G22" s="15">
-        <v>40469</v>
-      </c>
-      <c r="H22" s="14">
-        <v>84416</v>
-      </c>
-      <c r="I22" s="11">
-        <v>201</v>
-      </c>
-      <c r="J22" s="14">
-        <v>19189</v>
-      </c>
-      <c r="K22" s="11">
-        <v>806</v>
-      </c>
-      <c r="L22" s="19">
-        <v>20374</v>
-      </c>
-      <c r="M22" s="19">
-        <v>6999</v>
-      </c>
-      <c r="N22" s="19">
-        <v>9704</v>
-      </c>
-      <c r="O22" s="11">
-        <v>7166</v>
-      </c>
-      <c r="P22" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="Q22">
-        <v>25653</v>
-      </c>
-      <c r="R22" s="11">
-        <v>33350</v>
-      </c>
-      <c r="S22" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="T22">
-        <v>10130</v>
-      </c>
-      <c r="U22" s="11">
-        <v>8996</v>
-      </c>
-      <c r="V22" s="19"/>
-    </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>150</v>
       </c>
       <c r="B23" t="s">
         <v>98</v>
@@ -2724,38 +2703,104 @@
         <v>2.67</v>
       </c>
       <c r="D23" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="E23" s="14">
+        <v>4296</v>
+      </c>
+      <c r="F23" s="11">
+        <v>476</v>
+      </c>
+      <c r="G23" s="15">
+        <v>40469</v>
+      </c>
+      <c r="H23" s="14">
+        <v>84416</v>
+      </c>
+      <c r="I23" s="11">
+        <v>201</v>
+      </c>
+      <c r="J23" s="14">
+        <v>19189</v>
+      </c>
+      <c r="K23" s="11">
+        <v>806</v>
+      </c>
+      <c r="L23" s="19">
+        <v>20374</v>
+      </c>
+      <c r="M23" s="19">
+        <v>6999</v>
+      </c>
+      <c r="N23" s="19">
+        <v>9704</v>
+      </c>
+      <c r="O23" s="11">
+        <v>7166</v>
+      </c>
+      <c r="P23" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q23">
+        <v>25653</v>
+      </c>
+      <c r="R23" s="11">
+        <v>33350</v>
+      </c>
+      <c r="S23" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="T23">
+        <v>10130</v>
+      </c>
+      <c r="U23" s="11">
+        <v>8996</v>
+      </c>
+      <c r="V23" s="19"/>
+    </row>
+    <row r="24" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>150</v>
+      </c>
+      <c r="B24" t="s">
+        <v>98</v>
+      </c>
+      <c r="C24" s="7">
+        <v>2.67</v>
+      </c>
+      <c r="D24" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="E23" s="14"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="14">
+      <c r="E24" s="14"/>
+      <c r="F24" s="11"/>
+      <c r="G24" s="15"/>
+      <c r="H24" s="14"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="14">
         <v>23187</v>
       </c>
-      <c r="K23" s="11">
+      <c r="K24" s="11">
         <v>742</v>
       </c>
-      <c r="L23">
+      <c r="L24">
         <v>20211</v>
       </c>
-      <c r="M23">
+      <c r="M24">
         <v>6731</v>
       </c>
-      <c r="N23">
+      <c r="N24">
         <v>9800</v>
       </c>
-      <c r="O23" s="11">
+      <c r="O24" s="11">
         <v>7193</v>
       </c>
-      <c r="P23" s="8"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="8"/>
-      <c r="U23" s="11"/>
+      <c r="P24" s="8"/>
+      <c r="R24" s="11"/>
+      <c r="S24" s="8"/>
+      <c r="U24" s="11"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A19:V23">
+  <sortState ref="A19:V23">
     <sortCondition ref="V19:V23"/>
   </sortState>
   <mergeCells count="6">
@@ -2771,29 +2816,29 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9FE89E42-58B4-4FEF-A9D5-830DE33AE146}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.26953125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.1796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.42578125" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.453125" customWidth="1"/>
+    <col min="10" max="10" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7265625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.35">
       <c r="B1" s="9" t="s">
         <v>73</v>
       </c>
@@ -2843,7 +2888,7 @@
       <c r="V1" s="9"/>
       <c r="W1" s="9"/>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2863,7 +2908,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2880,7 +2925,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2897,7 +2942,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2917,7 +2962,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2949,7 +2994,7 @@
         <v>81396</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2978,7 +3023,7 @@
         <v>4516</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -3013,7 +3058,7 @@
         <v>26.43</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -3051,7 +3096,7 @@
         <v>35.35</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -3084,7 +3129,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L10">
+  <sortState ref="A2:L10">
     <sortCondition ref="A2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>